<commit_message>
overdue commit, creating datasets for thesis experiments and change the files to analyze experiments
</commit_message>
<xml_diff>
--- a/code/imputationExperiment/imputeCorrected.xlsx
+++ b/code/imputationExperiment/imputeCorrected.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maarten\Desktop\Afstuderen\thesis_stock_prediction_repo\code\imputationExperiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC377244-5905-4FAF-BABB-E346AE9F6987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBDB3C3-32D7-4344-8F20-421D0A31EB84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,9 +79,6 @@
     <t>["returns","single_run","20-step-ahead","20-predictions","2D-prediction","excluding_imputedvalues","seed4","minmax-11","4-year","shifted30"]</t>
   </si>
   <si>
-    <t>globalmean</t>
-  </si>
-  <si>
     <t>IM1-201</t>
   </si>
   <si>
@@ -745,9 +742,6 @@
     <t>["excluding_imputedvalues","shifted30","6D-prediction","4-year","20-predictions","seed4","minmax-11","single_run","20-step-ahead","returns"]</t>
   </si>
   <si>
-    <t>5_imputations_combined</t>
-  </si>
-  <si>
     <t>IM1-92</t>
   </si>
   <si>
@@ -1157,6 +1151,12 @@
   </si>
   <si>
     <t>smape</t>
+  </si>
+  <si>
+    <t>g_mean</t>
+  </si>
+  <si>
+    <t>combination_all</t>
   </si>
 </sst>
 </file>
@@ -2000,8 +2000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="H163" sqref="H163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,19 +2024,19 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="H1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="I1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2178,7 +2178,7 @@
         <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I6">
         <v>33</v>
@@ -2186,7 +2186,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1">
         <v>44390.667500000003</v>
@@ -2195,7 +2195,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -2215,7 +2215,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1">
         <v>44390.667210648149</v>
@@ -2224,7 +2224,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -2236,7 +2236,7 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8">
         <v>33</v>
@@ -2244,7 +2244,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1">
         <v>44390.667048611111</v>
@@ -2253,7 +2253,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1">
         <v>44390.666747685187</v>
@@ -2282,7 +2282,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -2302,7 +2302,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1">
         <v>44390.666527777779</v>
@@ -2311,7 +2311,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -2323,7 +2323,7 @@
         <v>7</v>
       </c>
       <c r="H11" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I11">
         <v>33</v>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>44390.665555555555</v>
@@ -2340,7 +2340,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -2360,7 +2360,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="1">
         <v>44390.665405092594</v>
@@ -2369,7 +2369,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13">
         <v>4</v>
@@ -2389,7 +2389,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1">
         <v>44390.664351851854</v>
@@ -2398,7 +2398,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14">
         <v>3</v>
@@ -2410,7 +2410,7 @@
         <v>7</v>
       </c>
       <c r="H14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I14">
         <v>33</v>
@@ -2418,7 +2418,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1">
         <v>44390.663900462961</v>
@@ -2427,7 +2427,7 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1">
         <v>44390.663888888892</v>
@@ -2456,7 +2456,7 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -2476,7 +2476,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1">
         <v>44390.663599537038</v>
@@ -2485,7 +2485,7 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -2505,7 +2505,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="1">
         <v>44390.663437499999</v>
@@ -2514,7 +2514,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -2534,7 +2534,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1">
         <v>44390.663437499999</v>
@@ -2543,7 +2543,7 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -2555,7 +2555,7 @@
         <v>7</v>
       </c>
       <c r="H19" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I19">
         <v>33</v>
@@ -2563,7 +2563,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1">
         <v>44390.662638888891</v>
@@ -2572,7 +2572,7 @@
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20">
         <v>3</v>
@@ -2592,7 +2592,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="1">
         <v>44390.662442129629</v>
@@ -2601,7 +2601,7 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E21">
         <v>3</v>
@@ -2621,7 +2621,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="1">
         <v>44390.661493055559</v>
@@ -2630,7 +2630,7 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22">
         <v>2</v>
@@ -2642,7 +2642,7 @@
         <v>7</v>
       </c>
       <c r="H22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I22">
         <v>33</v>
@@ -2650,7 +2650,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="1">
         <v>44390.66128472222</v>
@@ -2659,7 +2659,7 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E23">
         <v>3</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24" s="1">
         <v>44390.661122685182</v>
@@ -2688,7 +2688,7 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24">
         <v>4</v>
@@ -2700,7 +2700,7 @@
         <v>7</v>
       </c>
       <c r="H24" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I24">
         <v>90</v>
@@ -2708,7 +2708,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="1">
         <v>44390.660763888889</v>
@@ -2717,7 +2717,7 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -2737,7 +2737,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" s="1">
         <v>44390.660451388889</v>
@@ -2746,7 +2746,7 @@
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -2766,7 +2766,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27" s="1">
         <v>44390.66034722222</v>
@@ -2775,7 +2775,7 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -2787,7 +2787,7 @@
         <v>7</v>
       </c>
       <c r="H27" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I27">
         <v>33</v>
@@ -2795,7 +2795,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" s="1">
         <v>44390.66033564815</v>
@@ -2804,7 +2804,7 @@
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -2824,7 +2824,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" s="1">
         <v>44390.659826388888</v>
@@ -2833,7 +2833,7 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E29">
         <v>2</v>
@@ -2853,7 +2853,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B30" s="1">
         <v>44390.659467592595</v>
@@ -2862,7 +2862,7 @@
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E30">
         <v>2</v>
@@ -2882,7 +2882,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B31" s="1">
         <v>44390.659166666665</v>
@@ -2891,7 +2891,7 @@
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E31">
         <v>2</v>
@@ -2911,7 +2911,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="1">
         <v>44390.658715277779</v>
@@ -2920,7 +2920,7 @@
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -2932,7 +2932,7 @@
         <v>7</v>
       </c>
       <c r="H32" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I32">
         <v>90</v>
@@ -2940,7 +2940,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B33" s="1">
         <v>44390.658645833333</v>
@@ -2949,7 +2949,7 @@
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -2961,7 +2961,7 @@
         <v>7</v>
       </c>
       <c r="H33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I33">
         <v>33</v>
@@ -2969,7 +2969,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" s="1">
         <v>44390.65761574074</v>
@@ -2978,7 +2978,7 @@
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -2998,7 +2998,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B35" s="1">
         <v>44390.65724537037</v>
@@ -3007,7 +3007,7 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -3027,7 +3027,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36" s="1">
         <v>44390.657210648147</v>
@@ -3036,7 +3036,7 @@
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -3048,7 +3048,7 @@
         <v>7</v>
       </c>
       <c r="H36" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I36">
         <v>33</v>
@@ -3056,7 +3056,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B37" s="1">
         <v>44390.657083333332</v>
@@ -3065,7 +3065,7 @@
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -3085,7 +3085,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B38" s="1">
         <v>44390.657048611109</v>
@@ -3094,7 +3094,7 @@
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E38">
         <v>4</v>
@@ -3106,7 +3106,7 @@
         <v>7</v>
       </c>
       <c r="H38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I38">
         <v>90</v>
@@ -3114,7 +3114,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B39" s="1">
         <v>44390.657002314816</v>
@@ -3123,7 +3123,7 @@
         <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -3143,7 +3143,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B40" s="1">
         <v>44390.656701388885</v>
@@ -3152,7 +3152,7 @@
         <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E40">
         <v>4</v>
@@ -3161,7 +3161,7 @@
         <v>1.76455586391066E-2</v>
       </c>
       <c r="G40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H40" t="s">
         <v>8</v>
@@ -3172,7 +3172,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B41" s="1">
         <v>44390.656608796293</v>
@@ -3181,7 +3181,7 @@
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -3201,7 +3201,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B42" s="1">
         <v>44390.656319444446</v>
@@ -3210,7 +3210,7 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E42">
         <v>2</v>
@@ -3222,7 +3222,7 @@
         <v>7</v>
       </c>
       <c r="H42" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I42">
         <v>90</v>
@@ -3230,7 +3230,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B43" s="1">
         <v>44390.655729166669</v>
@@ -3239,7 +3239,7 @@
         <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -3251,7 +3251,7 @@
         <v>7</v>
       </c>
       <c r="H43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I43">
         <v>33</v>
@@ -3259,7 +3259,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B44" s="1">
         <v>44390.654953703706</v>
@@ -3268,7 +3268,7 @@
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E44">
         <v>3</v>
@@ -3280,7 +3280,7 @@
         <v>7</v>
       </c>
       <c r="H44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I44">
         <v>90</v>
@@ -3288,7 +3288,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B45" s="1">
         <v>44390.654849537037</v>
@@ -3297,7 +3297,7 @@
         <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -3317,7 +3317,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B46" s="1">
         <v>44390.654340277775</v>
@@ -3326,7 +3326,7 @@
         <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -3346,7 +3346,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B47" s="1">
         <v>44390.654282407406</v>
@@ -3355,7 +3355,7 @@
         <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E47">
         <v>4</v>
@@ -3364,7 +3364,7 @@
         <v>2.15695069248809E-2</v>
       </c>
       <c r="G47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H47" t="s">
         <v>13</v>
@@ -3375,7 +3375,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B48" s="1">
         <v>44390.653923611113</v>
@@ -3384,7 +3384,7 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -3396,7 +3396,7 @@
         <v>7</v>
       </c>
       <c r="H48" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I48">
         <v>90</v>
@@ -3404,7 +3404,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B49" s="1">
         <v>44390.653912037036</v>
@@ -3413,7 +3413,7 @@
         <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E49">
         <v>4</v>
@@ -3422,7 +3422,7 @@
         <v>3.54972238403208E-2</v>
       </c>
       <c r="G49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H49" t="s">
         <v>16</v>
@@ -3433,7 +3433,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B50" s="1">
         <v>44390.653854166667</v>
@@ -3442,7 +3442,7 @@
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E50">
         <v>4</v>
@@ -3451,10 +3451,10 @@
         <v>2.4917900724572499E-2</v>
       </c>
       <c r="G50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H50" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I50">
         <v>33</v>
@@ -3462,7 +3462,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B51" s="1">
         <v>44390.653738425928</v>
@@ -3471,7 +3471,7 @@
         <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -3491,7 +3491,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B52" s="1">
         <v>44390.653263888889</v>
@@ -3500,7 +3500,7 @@
         <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E52">
         <v>3</v>
@@ -3509,7 +3509,7 @@
         <v>1.97586992352436E-2</v>
       </c>
       <c r="G52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H52" t="s">
         <v>8</v>
@@ -3520,7 +3520,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B53" s="1">
         <v>44390.65284722222</v>
@@ -3529,7 +3529,7 @@
         <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E53">
         <v>2</v>
@@ -3541,7 +3541,7 @@
         <v>7</v>
       </c>
       <c r="H53" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I53">
         <v>90</v>
@@ -3549,7 +3549,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B54" s="1">
         <v>44390.652731481481</v>
@@ -3558,7 +3558,7 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E54">
         <v>4</v>
@@ -3567,10 +3567,10 @@
         <v>3.6071599441256097E-2</v>
       </c>
       <c r="G54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H54" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I54">
         <v>33</v>
@@ -3578,7 +3578,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B55" s="1">
         <v>44390.652094907404</v>
@@ -3587,7 +3587,7 @@
         <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E55">
         <v>4</v>
@@ -3596,7 +3596,7 @@
         <v>3.2938725719668799E-2</v>
       </c>
       <c r="G55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H55" t="s">
         <v>13</v>
@@ -3607,7 +3607,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B56" s="1">
         <v>44390.651898148149</v>
@@ -3616,7 +3616,7 @@
         <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E56">
         <v>4</v>
@@ -3625,7 +3625,7 @@
         <v>3.5722889566833303E-2</v>
       </c>
       <c r="G56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H56" t="s">
         <v>16</v>
@@ -3636,7 +3636,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B57" s="1">
         <v>44390.651469907411</v>
@@ -3645,7 +3645,7 @@
         <v>5</v>
       </c>
       <c r="D57" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -3657,7 +3657,7 @@
         <v>7</v>
       </c>
       <c r="H57" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I57">
         <v>90</v>
@@ -3665,7 +3665,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B58" s="1">
         <v>44390.651423611111</v>
@@ -3674,7 +3674,7 @@
         <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E58">
         <v>4</v>
@@ -3683,7 +3683,7 @@
         <v>3.8796554602299901E-2</v>
       </c>
       <c r="G58" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H58" t="s">
         <v>8</v>
@@ -3694,7 +3694,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B59" s="1">
         <v>44390.651134259257</v>
@@ -3703,7 +3703,7 @@
         <v>5</v>
       </c>
       <c r="D59" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E59">
         <v>3</v>
@@ -3712,7 +3712,7 @@
         <v>1.6593333714210401E-2</v>
       </c>
       <c r="G59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H59" t="s">
         <v>13</v>
@@ -3723,7 +3723,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B60" s="1">
         <v>44390.650775462964</v>
@@ -3732,7 +3732,7 @@
         <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E60">
         <v>3</v>
@@ -3741,7 +3741,7 @@
         <v>2.8747747967434199E-2</v>
       </c>
       <c r="G60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H60" t="s">
         <v>16</v>
@@ -3752,7 +3752,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B61" s="1">
         <v>44390.650752314818</v>
@@ -3761,7 +3761,7 @@
         <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -3773,7 +3773,7 @@
         <v>7</v>
       </c>
       <c r="H61" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I61">
         <v>90</v>
@@ -3781,7 +3781,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B62" s="1">
         <v>44390.650717592594</v>
@@ -3790,7 +3790,7 @@
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E62">
         <v>3</v>
@@ -3799,10 +3799,10 @@
         <v>2.1701874290447402E-2</v>
       </c>
       <c r="G62" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I62">
         <v>33</v>
@@ -3810,7 +3810,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B63" s="1">
         <v>44390.650625000002</v>
@@ -3819,7 +3819,7 @@
         <v>5</v>
       </c>
       <c r="D63" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E63">
         <v>4</v>
@@ -3828,10 +3828,10 @@
         <v>3.7815655654191802E-2</v>
       </c>
       <c r="G63" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H63" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I63">
         <v>90</v>
@@ -3839,7 +3839,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B64" s="1">
         <v>44390.649872685186</v>
@@ -3848,7 +3848,7 @@
         <v>5</v>
       </c>
       <c r="D64" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E64">
         <v>3</v>
@@ -3857,10 +3857,10 @@
         <v>3.6269758257573503E-2</v>
       </c>
       <c r="G64" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H64" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I64">
         <v>33</v>
@@ -3868,7 +3868,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B65" s="1">
         <v>44390.649826388886</v>
@@ -3877,7 +3877,7 @@
         <v>5</v>
       </c>
       <c r="D65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E65">
         <v>2</v>
@@ -3886,7 +3886,7 @@
         <v>1.53746873084295E-2</v>
       </c>
       <c r="G65" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H65" t="s">
         <v>8</v>
@@ -3897,7 +3897,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B66" s="1">
         <v>44390.649131944447</v>
@@ -3906,7 +3906,7 @@
         <v>5</v>
       </c>
       <c r="D66" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E66">
         <v>3</v>
@@ -3915,7 +3915,7 @@
         <v>3.2992490622337299E-2</v>
       </c>
       <c r="G66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H66" t="s">
         <v>13</v>
@@ -3926,7 +3926,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B67" s="1">
         <v>44390.648993055554</v>
@@ -3935,7 +3935,7 @@
         <v>5</v>
       </c>
       <c r="D67" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E67">
         <v>3</v>
@@ -3944,7 +3944,7 @@
         <v>3.5573779223556701E-2</v>
       </c>
       <c r="G67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H67" t="s">
         <v>16</v>
@@ -3955,7 +3955,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B68" s="1">
         <v>44390.648761574077</v>
@@ -3964,7 +3964,7 @@
         <v>5</v>
       </c>
       <c r="D68" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E68">
         <v>4</v>
@@ -3973,10 +3973,10 @@
         <v>3.5671628491148903E-2</v>
       </c>
       <c r="G68" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H68" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I68">
         <v>90</v>
@@ -3984,7 +3984,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B69" s="1">
         <v>44390.648680555554</v>
@@ -3993,7 +3993,7 @@
         <v>5</v>
       </c>
       <c r="D69" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E69">
         <v>3</v>
@@ -4002,7 +4002,7 @@
         <v>3.8605288318187901E-2</v>
       </c>
       <c r="G69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H69" t="s">
         <v>8</v>
@@ -4013,7 +4013,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B70" s="1">
         <v>44390.648587962962</v>
@@ -4022,7 +4022,7 @@
         <v>5</v>
       </c>
       <c r="D70" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -4034,7 +4034,7 @@
         <v>7</v>
       </c>
       <c r="H70" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I70">
         <v>90</v>
@@ -4042,7 +4042,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B71" s="1">
         <v>44390.647997685184</v>
@@ -4051,7 +4051,7 @@
         <v>5</v>
       </c>
       <c r="D71" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E71">
         <v>2</v>
@@ -4060,7 +4060,7 @@
         <v>1.65253140862462E-2</v>
       </c>
       <c r="G71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H71" t="s">
         <v>13</v>
@@ -4071,7 +4071,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B72" s="1">
         <v>44390.647766203707</v>
@@ -4080,7 +4080,7 @@
         <v>5</v>
       </c>
       <c r="D72" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E72">
         <v>3</v>
@@ -4089,10 +4089,10 @@
         <v>3.6610998789641899E-2</v>
       </c>
       <c r="G72" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H72" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I72">
         <v>90</v>
@@ -4100,7 +4100,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B73" s="1">
         <v>44390.647627314815</v>
@@ -4109,7 +4109,7 @@
         <v>5</v>
       </c>
       <c r="D73" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E73">
         <v>2</v>
@@ -4118,7 +4118,7 @@
         <v>2.1770115259626799E-2</v>
       </c>
       <c r="G73" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H73" t="s">
         <v>16</v>
@@ -4129,7 +4129,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B74" s="1">
         <v>44390.647569444445</v>
@@ -4138,7 +4138,7 @@
         <v>5</v>
       </c>
       <c r="D74" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E74">
         <v>2</v>
@@ -4147,10 +4147,10 @@
         <v>2.4001836402046402E-2</v>
       </c>
       <c r="G74" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H74" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I74">
         <v>33</v>
@@ -4158,7 +4158,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B75" s="1">
         <v>44390.647013888891</v>
@@ -4167,7 +4167,7 @@
         <v>5</v>
       </c>
       <c r="D75" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E75">
         <v>2</v>
@@ -4176,10 +4176,10 @@
         <v>1.7292446402932999E-2</v>
       </c>
       <c r="G75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H75" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I75">
         <v>33</v>
@@ -4187,7 +4187,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B76" s="1">
         <v>44390.64638888889</v>
@@ -4196,7 +4196,7 @@
         <v>5</v>
       </c>
       <c r="D76" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -4205,7 +4205,7 @@
         <v>1.3701157531174299E-2</v>
       </c>
       <c r="G76" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H76" t="s">
         <v>8</v>
@@ -4216,7 +4216,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B77" s="1">
         <v>44390.646365740744</v>
@@ -4225,7 +4225,7 @@
         <v>5</v>
       </c>
       <c r="D77" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E77">
         <v>3</v>
@@ -4234,10 +4234,10 @@
         <v>3.5820064104070397E-2</v>
       </c>
       <c r="G77" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H77" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I77">
         <v>90</v>
@@ -4245,7 +4245,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B78" s="1">
         <v>44390.646284722221</v>
@@ -4254,7 +4254,7 @@
         <v>5</v>
       </c>
       <c r="D78" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E78">
         <v>4</v>
@@ -4263,7 +4263,7 @@
         <v>3.0656824794011699E-2</v>
       </c>
       <c r="G78" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H78" t="s">
         <v>8</v>
@@ -4274,7 +4274,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B79" s="1">
         <v>44390.646249999998</v>
@@ -4283,7 +4283,7 @@
         <v>5</v>
       </c>
       <c r="D79" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E79">
         <v>4</v>
@@ -4292,7 +4292,7 @@
         <v>3.0875839316197199E-2</v>
       </c>
       <c r="G79" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H79" t="s">
         <v>13</v>
@@ -4303,7 +4303,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B80" s="1">
         <v>44390.646249999998</v>
@@ -4312,7 +4312,7 @@
         <v>5</v>
       </c>
       <c r="D80" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E80">
         <v>4</v>
@@ -4321,7 +4321,7 @@
         <v>4.5050571466066801E-2</v>
       </c>
       <c r="G80" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H80" t="s">
         <v>16</v>
@@ -4332,7 +4332,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B81" s="1">
         <v>44390.646168981482</v>
@@ -4341,7 +4341,7 @@
         <v>5</v>
       </c>
       <c r="D81" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E81">
         <v>2</v>
@@ -4350,7 +4350,7 @@
         <v>3.4785303341607801E-2</v>
       </c>
       <c r="G81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H81" t="s">
         <v>13</v>
@@ -4361,7 +4361,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B82" s="1">
         <v>44390.64607638889</v>
@@ -4370,7 +4370,7 @@
         <v>5</v>
       </c>
       <c r="D82" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E82">
         <v>2</v>
@@ -4379,7 +4379,7 @@
         <v>3.7288936603711999E-2</v>
       </c>
       <c r="G82" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H82" t="s">
         <v>16</v>
@@ -4390,7 +4390,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B83" s="1">
         <v>44390.645937499998</v>
@@ -4399,7 +4399,7 @@
         <v>5</v>
       </c>
       <c r="D83" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E83">
         <v>2</v>
@@ -4408,7 +4408,7 @@
         <v>3.9191987647798299E-2</v>
       </c>
       <c r="G83" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H83" t="s">
         <v>8</v>
@@ -4419,7 +4419,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B84" s="1">
         <v>44390.644849537035</v>
@@ -4428,7 +4428,7 @@
         <v>5</v>
       </c>
       <c r="D84" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E84">
         <v>1</v>
@@ -4437,7 +4437,7 @@
         <v>2.1689397912015702E-2</v>
       </c>
       <c r="G84" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H84" t="s">
         <v>13</v>
@@ -4448,7 +4448,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B85" s="1">
         <v>44390.644849537035</v>
@@ -4457,7 +4457,7 @@
         <v>5</v>
       </c>
       <c r="D85" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E85">
         <v>2</v>
@@ -4466,10 +4466,10 @@
         <v>3.7523782198114801E-2</v>
       </c>
       <c r="G85" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H85" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I85">
         <v>90</v>
@@ -4477,7 +4477,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B86" s="1">
         <v>44390.644490740742</v>
@@ -4486,7 +4486,7 @@
         <v>5</v>
       </c>
       <c r="D86" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -4495,7 +4495,7 @@
         <v>2.8687045373426701E-2</v>
       </c>
       <c r="G86" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H86" t="s">
         <v>16</v>
@@ -4506,7 +4506,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B87" s="1">
         <v>44390.644421296296</v>
@@ -4515,7 +4515,7 @@
         <v>5</v>
       </c>
       <c r="D87" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -4524,10 +4524,10 @@
         <v>1.62803991142824E-2</v>
       </c>
       <c r="G87" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H87" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I87">
         <v>33</v>
@@ -4535,7 +4535,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B88" s="1">
         <v>44390.644189814811</v>
@@ -4544,7 +4544,7 @@
         <v>5</v>
       </c>
       <c r="D88" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E88">
         <v>3</v>
@@ -4553,7 +4553,7 @@
         <v>2.6407194404597899E-2</v>
       </c>
       <c r="G88" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H88" t="s">
         <v>8</v>
@@ -4564,7 +4564,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B89" s="1">
         <v>44390.644155092596</v>
@@ -4573,7 +4573,7 @@
         <v>5</v>
       </c>
       <c r="D89" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -4582,10 +4582,10 @@
         <v>3.7025524606537498E-2</v>
       </c>
       <c r="G89" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H89" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I89">
         <v>33</v>
@@ -4593,7 +4593,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B90" s="1">
         <v>44390.644143518519</v>
@@ -4602,7 +4602,7 @@
         <v>5</v>
       </c>
       <c r="D90" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E90">
         <v>3</v>
@@ -4611,7 +4611,7 @@
         <v>2.82473728545574E-2</v>
       </c>
       <c r="G90" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H90" t="s">
         <v>13</v>
@@ -4622,7 +4622,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B91" s="1">
         <v>44390.644143518519</v>
@@ -4631,7 +4631,7 @@
         <v>5</v>
       </c>
       <c r="D91" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E91">
         <v>3</v>
@@ -4640,7 +4640,7 @@
         <v>5.5227864089313003E-2</v>
       </c>
       <c r="G91" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H91" t="s">
         <v>16</v>
@@ -4651,7 +4651,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B92" s="1">
         <v>44390.643969907411</v>
@@ -4660,7 +4660,7 @@
         <v>5</v>
       </c>
       <c r="D92" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E92">
         <v>2</v>
@@ -4669,10 +4669,10 @@
         <v>3.6895902208870499E-2</v>
       </c>
       <c r="G92" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H92" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I92">
         <v>90</v>
@@ -4680,7 +4680,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B93" s="1">
         <v>44390.643194444441</v>
@@ -4689,7 +4689,7 @@
         <v>5</v>
       </c>
       <c r="D93" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E93">
         <v>1</v>
@@ -4698,7 +4698,7 @@
         <v>3.75354683051616E-2</v>
       </c>
       <c r="G93" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H93" t="s">
         <v>8</v>
@@ -4709,7 +4709,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B94" s="1">
         <v>44390.643194444441</v>
@@ -4718,7 +4718,7 @@
         <v>5</v>
       </c>
       <c r="D94" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -4727,7 +4727,7 @@
         <v>3.3697692819649301E-2</v>
       </c>
       <c r="G94" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H94" t="s">
         <v>13</v>
@@ -4738,7 +4738,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B95" s="1">
         <v>44390.643171296295</v>
@@ -4747,7 +4747,7 @@
         <v>5</v>
       </c>
       <c r="D95" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E95">
         <v>1</v>
@@ -4756,7 +4756,7 @@
         <v>3.5470372577562102E-2</v>
       </c>
       <c r="G95" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H95" t="s">
         <v>16</v>
@@ -4767,7 +4767,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B96" s="1">
         <v>44390.642962962964</v>
@@ -4776,7 +4776,7 @@
         <v>5</v>
       </c>
       <c r="D96" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E96">
         <v>0</v>
@@ -4785,7 +4785,7 @@
         <v>2.0980444689097998E-2</v>
       </c>
       <c r="G96" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H96" t="s">
         <v>8</v>
@@ -4796,7 +4796,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B97" s="1">
         <v>44390.642094907409</v>
@@ -4805,7 +4805,7 @@
         <v>5</v>
       </c>
       <c r="D97" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E97">
         <v>2</v>
@@ -4814,7 +4814,7 @@
         <v>1.8457247736619199E-2</v>
       </c>
       <c r="G97" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H97" t="s">
         <v>8</v>
@@ -4825,7 +4825,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B98" s="1">
         <v>44390.642048611109</v>
@@ -4834,7 +4834,7 @@
         <v>5</v>
       </c>
       <c r="D98" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E98">
         <v>2</v>
@@ -4843,7 +4843,7 @@
         <v>4.0912418051000203E-2</v>
       </c>
       <c r="G98" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H98" t="s">
         <v>13</v>
@@ -4854,7 +4854,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B99" s="1">
         <v>44390.642048611109</v>
@@ -4863,7 +4863,7 @@
         <v>5</v>
       </c>
       <c r="D99" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E99">
         <v>2</v>
@@ -4872,7 +4872,7 @@
         <v>2.6119772635817599E-2</v>
       </c>
       <c r="G99" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H99" t="s">
         <v>16</v>
@@ -4883,7 +4883,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B100" s="1">
         <v>44390.64199074074</v>
@@ -4892,7 +4892,7 @@
         <v>5</v>
       </c>
       <c r="D100" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -4901,10 +4901,10 @@
         <v>3.5597179277275799E-2</v>
       </c>
       <c r="G100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H100" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I100">
         <v>90</v>
@@ -4912,7 +4912,7 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B101" s="1">
         <v>44390.641655092593</v>
@@ -4921,7 +4921,7 @@
         <v>5</v>
       </c>
       <c r="D101" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E101">
         <v>0</v>
@@ -4930,7 +4930,7 @@
         <v>2.5215841698702401E-2</v>
       </c>
       <c r="G101" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H101" t="s">
         <v>13</v>
@@ -4941,7 +4941,7 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B102" s="1">
         <v>44390.641585648147</v>
@@ -4950,7 +4950,7 @@
         <v>5</v>
       </c>
       <c r="D102" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E102">
         <v>1</v>
@@ -4959,10 +4959,10 @@
         <v>3.5940546791792399E-2</v>
       </c>
       <c r="G102" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H102" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I102">
         <v>90</v>
@@ -4970,7 +4970,7 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B103" s="1">
         <v>44390.641296296293</v>
@@ -4979,7 +4979,7 @@
         <v>5</v>
       </c>
       <c r="D103" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E103">
         <v>0</v>
@@ -4988,7 +4988,7 @@
         <v>3.6449955362771E-2</v>
       </c>
       <c r="G103" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H103" t="s">
         <v>16</v>
@@ -4999,7 +4999,7 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B104" s="1">
         <v>44390.641238425924</v>
@@ -5008,7 +5008,7 @@
         <v>5</v>
       </c>
       <c r="D104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E104">
         <v>0</v>
@@ -5017,10 +5017,10 @@
         <v>2.1501662258071898E-2</v>
       </c>
       <c r="G104" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H104" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I104">
         <v>33</v>
@@ -5028,7 +5028,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B105" s="1">
         <v>44390.641215277778</v>
@@ -5037,7 +5037,7 @@
         <v>5</v>
       </c>
       <c r="D105" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E105">
         <v>0</v>
@@ -5046,10 +5046,10 @@
         <v>2.0975218645081499E-2</v>
       </c>
       <c r="G105" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H105" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I105">
         <v>33</v>
@@ -5057,7 +5057,7 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B106" s="1">
         <v>44390.640405092592</v>
@@ -5066,7 +5066,7 @@
         <v>5</v>
       </c>
       <c r="D106" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E106">
         <v>0</v>
@@ -5075,7 +5075,7 @@
         <v>3.7531002961353498E-2</v>
       </c>
       <c r="G106" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H106" t="s">
         <v>8</v>
@@ -5086,7 +5086,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B107" s="1">
         <v>44390.640231481484</v>
@@ -5095,7 +5095,7 @@
         <v>5</v>
       </c>
       <c r="D107" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E107">
         <v>0</v>
@@ -5104,7 +5104,7 @@
         <v>3.3285146593324502E-2</v>
       </c>
       <c r="G107" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H107" t="s">
         <v>13</v>
@@ -5115,7 +5115,7 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B108" s="1">
         <v>44390.640196759261</v>
@@ -5124,7 +5124,7 @@
         <v>5</v>
       </c>
       <c r="D108" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E108">
         <v>0</v>
@@ -5133,7 +5133,7 @@
         <v>3.6110316454877701E-2</v>
       </c>
       <c r="G108" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H108" t="s">
         <v>16</v>
@@ -5144,7 +5144,7 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B109" s="1">
         <v>44390.639988425923</v>
@@ -5153,7 +5153,7 @@
         <v>5</v>
       </c>
       <c r="D109" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E109">
         <v>1</v>
@@ -5162,7 +5162,7 @@
         <v>2.9127261995113798E-2</v>
       </c>
       <c r="G109" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H109" t="s">
         <v>8</v>
@@ -5173,7 +5173,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B110" s="1">
         <v>44390.63994212963</v>
@@ -5182,7 +5182,7 @@
         <v>5</v>
       </c>
       <c r="D110" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E110">
         <v>1</v>
@@ -5191,7 +5191,7 @@
         <v>2.0413816409764401E-2</v>
       </c>
       <c r="G110" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H110" t="s">
         <v>13</v>
@@ -5202,7 +5202,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B111" s="1">
         <v>44390.63994212963</v>
@@ -5211,7 +5211,7 @@
         <v>5</v>
       </c>
       <c r="D111" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E111">
         <v>1</v>
@@ -5220,7 +5220,7 @@
         <v>2.22668104792536E-2</v>
       </c>
       <c r="G111" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H111" t="s">
         <v>16</v>
@@ -5231,7 +5231,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B112" s="1">
         <v>44390.639456018522</v>
@@ -5240,7 +5240,7 @@
         <v>5</v>
       </c>
       <c r="D112" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E112">
         <v>4</v>
@@ -5249,10 +5249,10 @@
         <v>4.4822485646439897E-2</v>
       </c>
       <c r="G112" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H112" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I112">
         <v>90</v>
@@ -5260,7 +5260,7 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B113" s="1">
         <v>44390.639120370368</v>
@@ -5269,7 +5269,7 @@
         <v>5</v>
       </c>
       <c r="D113" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E113">
         <v>0</v>
@@ -5278,10 +5278,10 @@
         <v>3.5790977592566699E-2</v>
       </c>
       <c r="G113" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H113" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I113">
         <v>90</v>
@@ -5289,7 +5289,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B114" s="1">
         <v>44390.639074074075</v>
@@ -5298,7 +5298,7 @@
         <v>5</v>
       </c>
       <c r="D114" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E114">
         <v>0</v>
@@ -5307,10 +5307,10 @@
         <v>3.6043692607638102E-2</v>
       </c>
       <c r="G114" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H114" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I114">
         <v>90</v>
@@ -5318,7 +5318,7 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B115" s="1">
         <v>44390.638275462959</v>
@@ -5327,7 +5327,7 @@
         <v>5</v>
       </c>
       <c r="D115" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E115">
         <v>4</v>
@@ -5336,10 +5336,10 @@
         <v>1.63636345031399E-2</v>
       </c>
       <c r="G115" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H115" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I115">
         <v>33</v>
@@ -5347,7 +5347,7 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B116" s="1">
         <v>44390.638229166667</v>
@@ -5356,7 +5356,7 @@
         <v>5</v>
       </c>
       <c r="D116" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E116">
         <v>4</v>
@@ -5365,10 +5365,10 @@
         <v>4.2544632100578801E-2</v>
       </c>
       <c r="G116" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H116" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I116">
         <v>33</v>
@@ -5376,7 +5376,7 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B117" s="1">
         <v>44390.637986111113</v>
@@ -5385,7 +5385,7 @@
         <v>5</v>
       </c>
       <c r="D117" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E117">
         <v>4</v>
@@ -5397,7 +5397,7 @@
         <v>7</v>
       </c>
       <c r="H117" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I117">
         <v>33</v>
@@ -5405,7 +5405,7 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B118" s="1">
         <v>44390.637939814813</v>
@@ -5414,7 +5414,7 @@
         <v>5</v>
       </c>
       <c r="D118" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E118">
         <v>4</v>
@@ -5423,10 +5423,10 @@
         <v>5.54317139083563E-2</v>
       </c>
       <c r="G118" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H118" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I118">
         <v>33</v>
@@ -5434,7 +5434,7 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B119" s="1">
         <v>44390.637835648151</v>
@@ -5443,7 +5443,7 @@
         <v>5</v>
       </c>
       <c r="D119" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E119">
         <v>0</v>
@@ -5452,7 +5452,7 @@
         <v>2.64366620622037E-2</v>
       </c>
       <c r="G119" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H119" t="s">
         <v>8</v>
@@ -5463,7 +5463,7 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B120" s="1">
         <v>44390.637777777774</v>
@@ -5472,7 +5472,7 @@
         <v>5</v>
       </c>
       <c r="D120" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E120">
         <v>0</v>
@@ -5481,7 +5481,7 @@
         <v>3.67581743807937E-2</v>
       </c>
       <c r="G120" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H120" t="s">
         <v>16</v>
@@ -5492,7 +5492,7 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B121" s="1">
         <v>44390.637777777774</v>
@@ -5501,7 +5501,7 @@
         <v>5</v>
       </c>
       <c r="D121" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E121">
         <v>0</v>
@@ -5510,7 +5510,7 @@
         <v>2.54494519284734E-2</v>
       </c>
       <c r="G121" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H121" t="s">
         <v>13</v>
@@ -5521,7 +5521,7 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B122" s="1">
         <v>44390.637465277781</v>
@@ -5530,7 +5530,7 @@
         <v>5</v>
       </c>
       <c r="D122" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E122">
         <v>4</v>
@@ -5539,10 +5539,10 @@
         <v>3.4956030128853802E-2</v>
       </c>
       <c r="G122" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H122" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I122">
         <v>90</v>
@@ -5550,7 +5550,7 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B123" s="1">
         <v>44390.637013888889</v>
@@ -5559,7 +5559,7 @@
         <v>5</v>
       </c>
       <c r="D123" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E123">
         <v>4</v>
@@ -5568,10 +5568,10 @@
         <v>3.48185103765579E-2</v>
       </c>
       <c r="G123" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H123" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I123">
         <v>90</v>
@@ -5579,7 +5579,7 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B124" s="1">
         <v>44390.636967592596</v>
@@ -5588,7 +5588,7 @@
         <v>5</v>
       </c>
       <c r="D124" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E124">
         <v>4</v>
@@ -5600,7 +5600,7 @@
         <v>7</v>
       </c>
       <c r="H124" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I124">
         <v>90</v>
@@ -5608,7 +5608,7 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B125" s="1">
         <v>44390.636493055557</v>
@@ -5617,7 +5617,7 @@
         <v>5</v>
       </c>
       <c r="D125" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E125">
         <v>4</v>
@@ -5626,7 +5626,7 @@
         <v>5.21694990102122E-2</v>
       </c>
       <c r="G125" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H125" t="s">
         <v>16</v>
@@ -5637,7 +5637,7 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B126" s="1">
         <v>44390.636122685188</v>
@@ -5646,7 +5646,7 @@
         <v>5</v>
       </c>
       <c r="D126" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E126">
         <v>3</v>
@@ -5655,10 +5655,10 @@
         <v>5.46887164466274E-2</v>
       </c>
       <c r="G126" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H126" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I126">
         <v>90</v>
@@ -5666,7 +5666,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B127" s="1">
         <v>44390.636087962965</v>
@@ -5675,7 +5675,7 @@
         <v>5</v>
       </c>
       <c r="D127" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E127">
         <v>4</v>
@@ -5684,10 +5684,10 @@
         <v>3.9024433910142702E-2</v>
       </c>
       <c r="G127" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H127" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I127">
         <v>90</v>
@@ -5695,7 +5695,7 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B128" s="1">
         <v>44390.635381944441</v>
@@ -5704,7 +5704,7 @@
         <v>5</v>
       </c>
       <c r="D128" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E128">
         <v>4</v>
@@ -5713,10 +5713,10 @@
         <v>2.35710288258036E-2</v>
       </c>
       <c r="G128" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H128" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I128">
         <v>33</v>
@@ -5724,7 +5724,7 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B129" s="1">
         <v>44390.635370370372</v>
@@ -5733,7 +5733,7 @@
         <v>5</v>
       </c>
       <c r="D129" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E129">
         <v>3</v>
@@ -5742,10 +5742,10 @@
         <v>5.2196149586519698E-2</v>
       </c>
       <c r="G129" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H129" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I129">
         <v>33</v>
@@ -5753,7 +5753,7 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B130" s="1">
         <v>44390.635312500002</v>
@@ -5762,7 +5762,7 @@
         <v>5</v>
       </c>
       <c r="D130" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E130">
         <v>4</v>
@@ -5771,7 +5771,7 @@
         <v>3.9157140942166498E-2</v>
       </c>
       <c r="G130" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H130" t="s">
         <v>13</v>
@@ -5782,7 +5782,7 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B131" s="1">
         <v>44390.635266203702</v>
@@ -5791,7 +5791,7 @@
         <v>5</v>
       </c>
       <c r="D131" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E131">
         <v>4</v>
@@ -5800,7 +5800,7 @@
         <v>2.2326865031027699E-2</v>
       </c>
       <c r="G131" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H131" t="s">
         <v>8</v>
@@ -5811,7 +5811,7 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B132" s="1">
         <v>44390.635011574072</v>
@@ -5820,7 +5820,7 @@
         <v>5</v>
       </c>
       <c r="D132" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E132">
         <v>3</v>
@@ -5829,10 +5829,10 @@
         <v>1.9210489503081199E-2</v>
       </c>
       <c r="G132" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H132" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I132">
         <v>33</v>
@@ -5840,7 +5840,7 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B133" s="1">
         <v>44390.634791666664</v>
@@ -5849,7 +5849,7 @@
         <v>5</v>
       </c>
       <c r="D133" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E133">
         <v>3</v>
@@ -5861,7 +5861,7 @@
         <v>7</v>
       </c>
       <c r="H133" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I133">
         <v>33</v>
@@ -5869,7 +5869,7 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B134" s="1">
         <v>44390.634780092594</v>
@@ -5878,7 +5878,7 @@
         <v>5</v>
       </c>
       <c r="D134" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E134">
         <v>3</v>
@@ -5887,10 +5887,10 @@
         <v>3.8322320337019697E-2</v>
       </c>
       <c r="G134" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H134" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I134">
         <v>33</v>
@@ -5898,7 +5898,7 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B135" s="1">
         <v>44390.634618055556</v>
@@ -5907,7 +5907,7 @@
         <v>5</v>
       </c>
       <c r="D135" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E135">
         <v>3</v>
@@ -5916,10 +5916,10 @@
         <v>5.3615360161912297E-2</v>
       </c>
       <c r="G135" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H135" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I135">
         <v>90</v>
@@ -5927,7 +5927,7 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B136" s="1">
         <v>44390.634039351855</v>
@@ -5936,7 +5936,7 @@
         <v>5</v>
       </c>
       <c r="D136" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E136">
         <v>3</v>
@@ -5945,7 +5945,7 @@
         <v>2.4995650209233399E-2</v>
       </c>
       <c r="G136" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H136" t="s">
         <v>16</v>
@@ -5956,7 +5956,7 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B137" s="1">
         <v>44390.633935185186</v>
@@ -5965,7 +5965,7 @@
         <v>5</v>
       </c>
       <c r="D137" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E137">
         <v>3</v>
@@ -5974,10 +5974,10 @@
         <v>3.5739918883785901E-2</v>
       </c>
       <c r="G137" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H137" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I137">
         <v>90</v>
@@ -5985,7 +5985,7 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B138" s="1">
         <v>44390.633877314816</v>
@@ -5994,7 +5994,7 @@
         <v>5</v>
       </c>
       <c r="D138" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E138">
         <v>3</v>
@@ -6006,7 +6006,7 @@
         <v>7</v>
       </c>
       <c r="H138" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I138">
         <v>90</v>
@@ -6014,7 +6014,7 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B139" s="1">
         <v>44390.633287037039</v>
@@ -6023,7 +6023,7 @@
         <v>5</v>
       </c>
       <c r="D139" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E139">
         <v>3</v>
@@ -6032,10 +6032,10 @@
         <v>3.6489319824546E-2</v>
       </c>
       <c r="G139" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H139" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I139">
         <v>90</v>
@@ -6043,7 +6043,7 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B140" s="1">
         <v>44390.633229166669</v>
@@ -6052,7 +6052,7 @@
         <v>5</v>
       </c>
       <c r="D140" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E140">
         <v>3</v>
@@ -6061,10 +6061,10 @@
         <v>3.77954431562533E-2</v>
       </c>
       <c r="G140" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H140" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I140">
         <v>33</v>
@@ -6072,7 +6072,7 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B141" s="1">
         <v>44390.633217592593</v>
@@ -6081,7 +6081,7 @@
         <v>5</v>
       </c>
       <c r="D141" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E141">
         <v>3</v>
@@ -6090,7 +6090,7 @@
         <v>3.8063017053823103E-2</v>
       </c>
       <c r="G141" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H141" t="s">
         <v>13</v>
@@ -6101,7 +6101,7 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B142" s="1">
         <v>44390.633171296293</v>
@@ -6110,7 +6110,7 @@
         <v>5</v>
       </c>
       <c r="D142" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E142">
         <v>3</v>
@@ -6119,7 +6119,7 @@
         <v>2.5169095480108102E-2</v>
       </c>
       <c r="G142" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H142" t="s">
         <v>8</v>
@@ -6130,7 +6130,7 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B143" s="1">
         <v>44390.632800925923</v>
@@ -6139,7 +6139,7 @@
         <v>5</v>
       </c>
       <c r="D143" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E143">
         <v>2</v>
@@ -6148,10 +6148,10 @@
         <v>3.2478176652951399E-2</v>
       </c>
       <c r="G143" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H143" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I143">
         <v>90</v>
@@ -6159,7 +6159,7 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B144" s="1">
         <v>44390.632511574076</v>
@@ -6168,7 +6168,7 @@
         <v>5</v>
       </c>
       <c r="D144" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E144">
         <v>2</v>
@@ -6177,10 +6177,10 @@
         <v>5.1148786872598398E-2</v>
       </c>
       <c r="G144" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H144" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I144">
         <v>33</v>
@@ -6188,7 +6188,7 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B145" s="1">
         <v>44390.63181712963</v>
@@ -6197,7 +6197,7 @@
         <v>5</v>
       </c>
       <c r="D145" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E145">
         <v>2</v>
@@ -6206,10 +6206,10 @@
         <v>3.6725302838665201E-2</v>
       </c>
       <c r="G145" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H145" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I145">
         <v>90</v>
@@ -6217,7 +6217,7 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B146" s="1">
         <v>44390.63175925926</v>
@@ -6226,7 +6226,7 @@
         <v>5</v>
       </c>
       <c r="D146" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E146">
         <v>2</v>
@@ -6235,10 +6235,10 @@
         <v>1.7822139557826699E-2</v>
       </c>
       <c r="G146" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H146" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I146">
         <v>33</v>
@@ -6246,7 +6246,7 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B147" s="1">
         <v>44390.631643518522</v>
@@ -6255,7 +6255,7 @@
         <v>5</v>
       </c>
       <c r="D147" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E147">
         <v>2</v>
@@ -6264,7 +6264,7 @@
         <v>3.11135965890568E-2</v>
       </c>
       <c r="G147" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H147" t="s">
         <v>16</v>
@@ -6275,7 +6275,7 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B148" s="1">
         <v>44390.631585648145</v>
@@ -6284,7 +6284,7 @@
         <v>5</v>
       </c>
       <c r="D148" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E148">
         <v>2</v>
@@ -6296,7 +6296,7 @@
         <v>7</v>
       </c>
       <c r="H148" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I148">
         <v>33</v>
@@ -6304,7 +6304,7 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B149" s="1">
         <v>44390.631585648145</v>
@@ -6313,7 +6313,7 @@
         <v>5</v>
       </c>
       <c r="D149" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E149">
         <v>2</v>
@@ -6322,10 +6322,10 @@
         <v>4.0265130723718699E-2</v>
       </c>
       <c r="G149" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H149" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I149">
         <v>33</v>
@@ -6333,7 +6333,7 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B150" s="1">
         <v>44390.631064814814</v>
@@ -6342,7 +6342,7 @@
         <v>5</v>
       </c>
       <c r="D150" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E150">
         <v>2</v>
@@ -6351,7 +6351,7 @@
         <v>4.4486147080823497E-2</v>
       </c>
       <c r="G150" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H150" t="s">
         <v>13</v>
@@ -6362,7 +6362,7 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B151" s="1">
         <v>44390.631064814814</v>
@@ -6371,7 +6371,7 @@
         <v>5</v>
       </c>
       <c r="D151" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E151">
         <v>2</v>
@@ -6380,10 +6380,10 @@
         <v>3.4828821114515802E-2</v>
       </c>
       <c r="G151" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H151" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I151">
         <v>33</v>
@@ -6391,7 +6391,7 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B152" s="1">
         <v>44390.631064814814</v>
@@ -6400,7 +6400,7 @@
         <v>5</v>
       </c>
       <c r="D152" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E152">
         <v>2</v>
@@ -6409,7 +6409,7 @@
         <v>2.4329129366072899E-2</v>
       </c>
       <c r="G152" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H152" t="s">
         <v>8</v>
@@ -6420,7 +6420,7 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B153" s="1">
         <v>44390.630844907406</v>
@@ -6429,7 +6429,7 @@
         <v>5</v>
       </c>
       <c r="D153" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E153">
         <v>2</v>
@@ -6441,7 +6441,7 @@
         <v>7</v>
       </c>
       <c r="H153" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I153">
         <v>90</v>
@@ -6449,7 +6449,7 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B154" s="1">
         <v>44390.630844907406</v>
@@ -6458,7 +6458,7 @@
         <v>5</v>
       </c>
       <c r="D154" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E154">
         <v>2</v>
@@ -6467,10 +6467,10 @@
         <v>3.47758730348511E-2</v>
       </c>
       <c r="G154" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H154" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I154">
         <v>90</v>
@@ -6478,7 +6478,7 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B155" s="1">
         <v>44390.630486111113</v>
@@ -6487,7 +6487,7 @@
         <v>5</v>
       </c>
       <c r="D155" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E155">
         <v>2</v>
@@ -6496,10 +6496,10 @@
         <v>4.3219911577969297E-2</v>
       </c>
       <c r="G155" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H155" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I155">
         <v>90</v>
@@ -6507,7 +6507,7 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B156" s="1">
         <v>44390.629664351851</v>
@@ -6516,7 +6516,7 @@
         <v>5</v>
       </c>
       <c r="D156" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E156">
         <v>1</v>
@@ -6525,10 +6525,10 @@
         <v>2.1985983605171101E-2</v>
       </c>
       <c r="G156" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H156" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I156">
         <v>33</v>
@@ -6536,7 +6536,7 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B157" s="1">
         <v>44390.629479166666</v>
@@ -6545,7 +6545,7 @@
         <v>5</v>
       </c>
       <c r="D157" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E157">
         <v>1</v>
@@ -6554,10 +6554,10 @@
         <v>6.74876358965905E-2</v>
       </c>
       <c r="G157" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H157" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I157">
         <v>90</v>
@@ -6565,7 +6565,7 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B158" s="1">
         <v>44390.629247685189</v>
@@ -6574,7 +6574,7 @@
         <v>5</v>
       </c>
       <c r="D158" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E158">
         <v>1</v>
@@ -6583,7 +6583,7 @@
         <v>3.7275410317827003E-2</v>
       </c>
       <c r="G158" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H158" t="s">
         <v>16</v>
@@ -6594,7 +6594,7 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B159" s="1">
         <v>44390.629016203704</v>
@@ -6603,7 +6603,7 @@
         <v>5</v>
       </c>
       <c r="D159" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E159">
         <v>1</v>
@@ -6612,10 +6612,10 @@
         <v>4.0483228768822703E-2</v>
       </c>
       <c r="G159" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H159" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I159">
         <v>90</v>
@@ -6623,7 +6623,7 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B160" s="1">
         <v>44390.628958333335</v>
@@ -6632,7 +6632,7 @@
         <v>5</v>
       </c>
       <c r="D160" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E160">
         <v>1</v>
@@ -6641,7 +6641,7 @@
         <v>4.08734085992392E-2</v>
       </c>
       <c r="G160" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H160" t="s">
         <v>13</v>
@@ -6652,7 +6652,7 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B161" s="1">
         <v>44390.628958333335</v>
@@ -6661,7 +6661,7 @@
         <v>5</v>
       </c>
       <c r="D161" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E161">
         <v>1</v>
@@ -6670,7 +6670,7 @@
         <v>2.9709917783900499E-2</v>
       </c>
       <c r="G161" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H161" t="s">
         <v>8</v>
@@ -6681,7 +6681,7 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B162" s="1">
         <v>44390.628958333335</v>
@@ -6690,7 +6690,7 @@
         <v>5</v>
       </c>
       <c r="D162" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E162">
         <v>1</v>
@@ -6699,10 +6699,10 @@
         <v>2.2024530012524399E-2</v>
       </c>
       <c r="G162" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H162" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I162">
         <v>33</v>
@@ -6710,7 +6710,7 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B163" s="1">
         <v>44390.628553240742</v>
@@ -6719,7 +6719,7 @@
         <v>5</v>
       </c>
       <c r="D163" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E163">
         <v>1</v>
@@ -6728,10 +6728,10 @@
         <v>1.97368329490538E-2</v>
       </c>
       <c r="G163" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H163" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I163">
         <v>33</v>
@@ -6739,7 +6739,7 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B164" s="1">
         <v>44390.628495370373</v>
@@ -6748,7 +6748,7 @@
         <v>5</v>
       </c>
       <c r="D164" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E164">
         <v>1</v>
@@ -6757,10 +6757,10 @@
         <v>2.4634962613919901E-2</v>
       </c>
       <c r="G164" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H164" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I164">
         <v>33</v>
@@ -6768,7 +6768,7 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B165" s="1">
         <v>44390.628495370373</v>
@@ -6777,7 +6777,7 @@
         <v>5</v>
       </c>
       <c r="D165" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E165">
         <v>1</v>
@@ -6789,7 +6789,7 @@
         <v>7</v>
       </c>
       <c r="H165" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I165">
         <v>33</v>
@@ -6797,7 +6797,7 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B166" s="1">
         <v>44390.627870370372</v>
@@ -6806,7 +6806,7 @@
         <v>5</v>
       </c>
       <c r="D166" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E166">
         <v>1</v>
@@ -6818,7 +6818,7 @@
         <v>7</v>
       </c>
       <c r="H166" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I166">
         <v>90</v>
@@ -6826,7 +6826,7 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B167" s="1">
         <v>44390.627870370372</v>
@@ -6835,7 +6835,7 @@
         <v>5</v>
       </c>
       <c r="D167" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E167">
         <v>1</v>
@@ -6844,10 +6844,10 @@
         <v>3.4685648782350198E-2</v>
       </c>
       <c r="G167" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H167" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I167">
         <v>90</v>
@@ -6855,7 +6855,7 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B168" s="1">
         <v>44390.627685185187</v>
@@ -6864,7 +6864,7 @@
         <v>5</v>
       </c>
       <c r="D168" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E168">
         <v>1</v>
@@ -6873,10 +6873,10 @@
         <v>5.7944842808494698E-2</v>
       </c>
       <c r="G168" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H168" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I168">
         <v>90</v>
@@ -6884,7 +6884,7 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B169" s="1">
         <v>44390.626747685186</v>
@@ -6893,7 +6893,7 @@
         <v>5</v>
       </c>
       <c r="D169" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E169">
         <v>0</v>
@@ -6902,10 +6902,10 @@
         <v>4.8699066295499499E-2</v>
       </c>
       <c r="G169" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H169" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I169">
         <v>33</v>
@@ -6913,7 +6913,7 @@
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B170" s="1">
         <v>44390.626736111109</v>
@@ -6922,7 +6922,7 @@
         <v>5</v>
       </c>
       <c r="D170" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E170">
         <v>0</v>
@@ -6931,7 +6931,7 @@
         <v>2.9938482218012999E-2</v>
       </c>
       <c r="G170" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H170" t="s">
         <v>16</v>
@@ -6942,7 +6942,7 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B171" s="1">
         <v>44390.626736111109</v>
@@ -6951,7 +6951,7 @@
         <v>5</v>
       </c>
       <c r="D171" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E171">
         <v>0</v>
@@ -6960,7 +6960,7 @@
         <v>2.37023696824595E-2</v>
       </c>
       <c r="G171" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H171" t="s">
         <v>8</v>
@@ -6971,7 +6971,7 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B172" s="1">
         <v>44390.626736111109</v>
@@ -6980,7 +6980,7 @@
         <v>5</v>
       </c>
       <c r="D172" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E172">
         <v>0</v>
@@ -6989,7 +6989,7 @@
         <v>4.0676516145123798E-2</v>
       </c>
       <c r="G172" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H172" t="s">
         <v>13</v>
@@ -7000,7 +7000,7 @@
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B173" s="1">
         <v>44390.626736111109</v>
@@ -7009,7 +7009,7 @@
         <v>5</v>
       </c>
       <c r="D173" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E173">
         <v>0</v>
@@ -7018,10 +7018,10 @@
         <v>1.86120127557611E-2</v>
       </c>
       <c r="G173" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H173" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I173">
         <v>33</v>
@@ -7029,7 +7029,7 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B174" s="1">
         <v>44390.626157407409</v>
@@ -7038,7 +7038,7 @@
         <v>5</v>
       </c>
       <c r="D174" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E174">
         <v>0</v>
@@ -7047,10 +7047,10 @@
         <v>3.5925555804288398E-2</v>
       </c>
       <c r="G174" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H174" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I174">
         <v>90</v>
@@ -7058,7 +7058,7 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B175" s="1">
         <v>44390.626157407409</v>
@@ -7067,7 +7067,7 @@
         <v>5</v>
       </c>
       <c r="D175" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E175">
         <v>0</v>
@@ -7076,10 +7076,10 @@
         <v>4.4645249210716199E-2</v>
       </c>
       <c r="G175" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H175" t="s">
-        <v>19</v>
+        <v>377</v>
       </c>
       <c r="I175">
         <v>90</v>
@@ -7087,7 +7087,7 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B176" s="1">
         <v>44390.625347222223</v>
@@ -7096,7 +7096,7 @@
         <v>5</v>
       </c>
       <c r="D176" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E176">
         <v>0</v>
@@ -7108,7 +7108,7 @@
         <v>7</v>
       </c>
       <c r="H176" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I176">
         <v>33</v>
@@ -7116,7 +7116,7 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B177" s="1">
         <v>44390.625347222223</v>
@@ -7125,7 +7125,7 @@
         <v>5</v>
       </c>
       <c r="D177" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E177">
         <v>0</v>
@@ -7134,10 +7134,10 @@
         <v>1.9791443400791101E-2</v>
       </c>
       <c r="G177" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H177" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I177">
         <v>33</v>
@@ -7145,7 +7145,7 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B178" s="1">
         <v>44390.625347222223</v>
@@ -7154,7 +7154,7 @@
         <v>5</v>
       </c>
       <c r="D178" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E178">
         <v>0</v>
@@ -7163,10 +7163,10 @@
         <v>3.0868354167945599E-2</v>
       </c>
       <c r="G178" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H178" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I178">
         <v>33</v>
@@ -7174,7 +7174,7 @@
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B179" s="1">
         <v>44390.624837962961</v>
@@ -7183,7 +7183,7 @@
         <v>5</v>
       </c>
       <c r="D179" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E179">
         <v>0</v>
@@ -7195,7 +7195,7 @@
         <v>7</v>
       </c>
       <c r="H179" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I179">
         <v>90</v>
@@ -7203,7 +7203,7 @@
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B180" s="1">
         <v>44390.624837962961</v>
@@ -7212,7 +7212,7 @@
         <v>5</v>
       </c>
       <c r="D180" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E180">
         <v>0</v>
@@ -7221,10 +7221,10 @@
         <v>3.5392235521248899E-2</v>
       </c>
       <c r="G180" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H180" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I180">
         <v>90</v>
@@ -7232,7 +7232,7 @@
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B181" s="1">
         <v>44390.624826388892</v>
@@ -7241,7 +7241,7 @@
         <v>5</v>
       </c>
       <c r="D181" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E181">
         <v>0</v>
@@ -7250,10 +7250,10 @@
         <v>4.6589734447693799E-2</v>
       </c>
       <c r="G181" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H181" t="s">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="I181">
         <v>90</v>

</xml_diff>